<commit_message>
Se termina la pantalla de solicitud en cocina. se corrigen bug de: Se pueden modificar pedidos en estado pendiente. No se pueden modificar solicitudes no seleccionadas. No se pueden crear materia primas vacias. Se modifica el archivo informacion para avances.
</commit_message>
<xml_diff>
--- a/Documentación/Info para Avances.xlsx
+++ b/Documentación/Info para Avances.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="60">
   <si>
     <t>Referencia</t>
   </si>
@@ -184,6 +184,18 @@
   </si>
   <si>
     <t>hay que retocar porque en si ya estaban</t>
+  </si>
+  <si>
+    <t>crear materiaprima</t>
+  </si>
+  <si>
+    <t>solo se pueden crear no se pueden ni eliminar ni modificar</t>
+  </si>
+  <si>
+    <t>todas las materia primas</t>
+  </si>
+  <si>
+    <t>nicof</t>
   </si>
 </sst>
 </file>
@@ -634,7 +646,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -782,28 +794,28 @@
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="1:4" ht="15" customHeight="1" thickBot="1">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="7" t="s">
         <v>28</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D12" s="10" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15" customHeight="1" thickBot="1">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="7" t="s">
         <v>30</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D13" s="11"/>
     </row>
@@ -979,17 +991,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="53.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
@@ -1019,6 +1031,23 @@
         <v>52</v>
       </c>
     </row>
+    <row r="2" spans="1:7">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2" t="s">
+        <v>59</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>